<commit_message>
project CRUD is done with validations
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ask for room</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>induction manual</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>ici is getting update to ck(an already exiting prj)</t>
+  </si>
+  <si>
+    <t>code commit</t>
   </si>
 </sst>
 </file>
@@ -375,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -386,22 +395,25 @@
     <col min="1" max="1" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -409,14 +421,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
employee CRUD migrated to generic CRUD implementation
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ask for room</t>
   </si>
@@ -39,13 +39,7 @@
     <t>induction manual</t>
   </si>
   <si>
-    <t>update</t>
-  </si>
-  <si>
-    <t>ici is getting update to ck(an already exiting prj)</t>
-  </si>
-  <si>
-    <t>code commit</t>
+    <t>validate collectionsName in server</t>
   </si>
 </sst>
 </file>
@@ -384,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -395,25 +389,22 @@
     <col min="1" max="1" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -421,24 +412,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G8" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>